<commit_message>
Added dynamic dropdows for commitment
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distribution_payments.xlsx
+++ b/public/sample_uploads/capital_distribution_payments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D76212-8176-4A5A-A1AD-30E64D1DCD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524B8EC2-69A3-419A-88BF-6537F240EF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Completed</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Payment Date *</t>
+  </si>
+  <si>
+    <t>Folio No</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -435,7 +438,7 @@
     <col min="6" max="6" width="13.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -454,8 +457,11 @@
       <c r="F1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -475,7 +481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -495,7 +501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -515,7 +521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -535,7 +541,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -555,7 +561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Fixed import of CDP to include cost of investment
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distribution_payments.xlsx
+++ b/public/sample_uploads/capital_distribution_payments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524B8EC2-69A3-419A-88BF-6537F240EF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C874BA8-77C5-49CB-929E-9CE697F2C604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Completed</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Folio No</t>
+  </si>
+  <si>
+    <t>Cost Of Investment *</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -434,11 +437,12 @@
     <col min="2" max="2" width="28.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.625" customWidth="1"/>
     <col min="4" max="4" width="18.6875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6875" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -452,16 +456,19 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -474,14 +481,17 @@
       <c r="D2" s="2">
         <v>194337</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F2" s="1">
         <v>44573</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -494,14 +504,17 @@
       <c r="D3" s="2">
         <v>249777</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
+        <v>200000</v>
+      </c>
+      <c r="F3" s="1">
         <v>44573</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -514,14 +527,17 @@
       <c r="D4" s="2">
         <v>148005</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
+        <v>90000</v>
+      </c>
+      <c r="F4" s="1">
         <v>44573</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -534,14 +550,17 @@
       <c r="D5" s="2">
         <v>175824</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F5" s="1">
         <v>44573</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -554,14 +573,17 @@
       <c r="D6" s="2">
         <v>222057</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
+        <v>200000</v>
+      </c>
+      <c r="F6" s="1">
         <v>44573</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -574,10 +596,13 @@
       <c r="D7" s="2">
         <v>236907</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
+        <v>200000</v>
+      </c>
+      <c r="F7" s="1">
         <v>44573</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Capital Distribution payment tests and checks (#471)
* Added tests for CDP import

* Added tests for CDP import
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distribution_payments.xlsx
+++ b/public/sample_uploads/capital_distribution_payments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseem Karmali\Desktop\bulk files with notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CE925A-145A-4585-9D8B-F147464D1E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9715CA49-56E0-4206-AC6C-AD8C4DA2F33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalDistrbutionPayment" sheetId="1" r:id="rId1"/>
@@ -236,41 +236,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Completed</t>
   </si>
   <si>
-    <t>Agri Fund</t>
-  </si>
-  <si>
-    <t>Sekhsaria family office</t>
-  </si>
-  <si>
-    <t>Bansal family office</t>
-  </si>
-  <si>
-    <t>Metta investors</t>
-  </si>
-  <si>
-    <t>Arun Gupta</t>
-  </si>
-  <si>
-    <t>Delta Ventures</t>
-  </si>
-  <si>
-    <t>Waterfield Advisors</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Distribution from Sale</t>
-  </si>
-  <si>
     <t>Fund *</t>
   </si>
   <si>
@@ -290,13 +266,40 @@
   </si>
   <si>
     <t>Cost Of Investment *</t>
+  </si>
+  <si>
+    <t>Distribution 1</t>
+  </si>
+  <si>
+    <t>Distribution 2</t>
+  </si>
+  <si>
+    <t>SAAS Fund</t>
+  </si>
+  <si>
+    <t>Investor 1</t>
+  </si>
+  <si>
+    <t>Investor 2</t>
+  </si>
+  <si>
+    <t>Investor 3</t>
+  </si>
+  <si>
+    <t>Investor 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution 1     </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -339,6 +342,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -366,19 +381,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{B8533CD2-A72C-410A-BCF1-DCC714EF7A20}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{FD314E3D-5FDA-4487-AD0C-DC4AFE842FE0}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{207E7983-3FC3-4F96-9EBF-4ECF842EB65F}"/>
+    <cellStyle name="Normal 5" xfId="1" xr:uid="{77FA2981-ECE6-4700-926C-1FA97F87A7A3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -693,7 +717,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -711,39 +735,39 @@
   <sheetData>
     <row r="1" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3">
         <v>194337</v>
@@ -755,18 +779,21 @@
         <v>44896</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3">
         <v>249777</v>
@@ -778,15 +805,18 @@
         <v>44896</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -801,15 +831,18 @@
         <v>44896</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -824,18 +857,21 @@
         <v>44896</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3">
         <v>222057</v>
@@ -847,18 +883,21 @@
         <v>44896</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3">
         <v>236907</v>
@@ -870,7 +909,10 @@
         <v>44896</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added download to remittances, disabled payment fields
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distribution_payments.xlsx
+++ b/public/sample_uploads/capital_distribution_payments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B77643-C79F-4404-944E-D4C4CCACCD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB22E3CF-6F07-42F8-A97E-A7D85FB02205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="735" windowWidth="23985" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{400AD210-7CD4-4E07-98A6-E4750893E185}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{400AD210-7CD4-4E07-98A6-E4750893E185}">
       <text>
         <r>
           <rPr>
@@ -182,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{368C02A8-283C-49DE-A429-73E906D5D0C3}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{368C02A8-283C-49DE-A429-73E906D5D0C3}">
       <text>
         <r>
           <rPr>
@@ -206,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{EE332C3D-65D0-4A0B-A67A-DD6759627668}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{EE332C3D-65D0-4A0B-A67A-DD6759627668}">
       <text>
         <r>
           <rPr>
@@ -236,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Completed</t>
   </si>
@@ -262,9 +262,6 @@
     <t>Folio No</t>
   </si>
   <si>
-    <t>Cost Of Investment *</t>
-  </si>
-  <si>
     <t>Distribution 1</t>
   </si>
   <si>
@@ -293,6 +290,12 @@
   </si>
   <si>
     <t>Income *</t>
+  </si>
+  <si>
+    <t>Face Value For Redemption *</t>
+  </si>
+  <si>
+    <t>Reinvestment</t>
   </si>
 </sst>
 </file>
@@ -714,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F3" sqref="F3:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -727,13 +730,14 @@
     <col min="3" max="3" width="18.3125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.1875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.4375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="2"/>
+    <col min="6" max="6" width="17.4375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.3125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -744,30 +748,33 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3">
         <v>194337</v>
@@ -775,25 +782,28 @@
       <c r="E2" s="3">
         <v>100000</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G2" s="4">
         <v>44896</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3">
         <v>249777</v>
@@ -801,25 +811,28 @@
       <c r="E3" s="3">
         <v>200000</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="4">
         <v>44896</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3">
         <v>148005</v>
@@ -827,25 +840,28 @@
       <c r="E4" s="3">
         <v>90000</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="4">
         <v>44896</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3">
         <v>175824</v>
@@ -853,25 +869,28 @@
       <c r="E5" s="3">
         <v>100000</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="4">
         <v>44896</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3">
         <v>222057</v>
@@ -879,25 +898,28 @@
       <c r="E6" s="3">
         <v>200000</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G6" s="4">
         <v>44896</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3">
         <v>236907</v>
@@ -905,82 +927,92 @@
       <c r="E7" s="3">
         <v>200000</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G7" s="4">
         <v>44896</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="G9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="4"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="F10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="F11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="F12" s="5"/>
+      <c r="G12" s="4"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="F13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="I13"/>
+    </row>
+    <row r="14" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
-      <c r="H15"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="I15"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{401D07CA-90D6-4C96-B53C-38E6383AFD3F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{401D07CA-90D6-4C96-B53C-38E6383AFD3F}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>